<commit_message>
Add few more testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/saucedemo.xlsx
+++ b/src/test/resources/testdata/saucedemo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Selenium Project\com.qa.saucedemo\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bosed\git\com.qa.saucedemo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC504F2-5484-4D9F-B4BC-5F7DB9D3E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F863B90-7EA6-40A6-B2DE-766BF57E1A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7430" yWindow="990" windowWidth="11110" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4850" yWindow="1350" windowWidth="11110" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>standard_user</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>error_user</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -78,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,56 +364,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>